<commit_message>
Add testing portfolios for scanning for sale portfolios
</commit_message>
<xml_diff>
--- a/purchased/account-ids.xlsx
+++ b/purchased/account-ids.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bpa/Desktop/latest-pull/test_purchased/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bpa/Desktop/projects/personal/consumer-debt-portfolio-cleaner/purchased/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26EAAA69-E982-1A47-86F0-866434A66354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A71508-B22E-6E43-A0CB-CE8F00967393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16440" xr2:uid="{241E207C-5F1E-134E-AA74-3CF2AB0C2EB3}"/>
   </bookViews>
@@ -32,100 +32,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>account</t>
-  </si>
-  <si>
-    <t>dumy</t>
-  </si>
-  <si>
-    <t>dumm2</t>
-  </si>
-  <si>
-    <t>jjffff</t>
-  </si>
-  <si>
-    <t>jfjjjd</t>
-  </si>
-  <si>
-    <t>hfhhfhf</t>
-  </si>
-  <si>
-    <t>jdjdjjf</t>
-  </si>
-  <si>
-    <t>dhdhfhf</t>
-  </si>
-  <si>
-    <t>dfjffjf</t>
-  </si>
-  <si>
-    <t>jdjjfjf</t>
-  </si>
-  <si>
-    <t>hdhdhd</t>
-  </si>
-  <si>
-    <t>fhfef</t>
-  </si>
-  <si>
-    <t>sjdjjdjk</t>
-  </si>
-  <si>
-    <t>jekekf</t>
-  </si>
-  <si>
-    <t>sjsjdjjde</t>
-  </si>
-  <si>
-    <t>jdjjfjee</t>
-  </si>
-  <si>
-    <t>ddeeue</t>
-  </si>
-  <si>
-    <t>sskeee</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>fg</t>
-  </si>
-  <si>
-    <t>grr</t>
-  </si>
-  <si>
-    <t>esskkf</t>
-  </si>
-  <si>
-    <t>ee</t>
-  </si>
-  <si>
-    <t>ff</t>
-  </si>
-  <si>
-    <t>fiirir</t>
-  </si>
-  <si>
-    <t>jddkd</t>
-  </si>
-  <si>
-    <t>dddkkd</t>
-  </si>
-  <si>
-    <t>djdjjdd</t>
+    <t>accountid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,166 +394,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2C5053-F3F1-4E46-83B1-12767E4FD0C1}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>300</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>301</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>456789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>456790</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>302</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>303</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>456791</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>456792</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>304</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>305</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>456793</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>456794</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>500</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>501</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>456795</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>456796</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>502</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>503</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>456797</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>456798</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>504</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>505</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>456799</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>456800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>506</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
+        <v>456801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>456802</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>456803</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>456804</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>456805</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>456806</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>456807</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>456808</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>456809</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>456810</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>456811</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>456812</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>456813</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>456814</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>456815</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>456816</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>456817</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>456818</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>456819</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>456820</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>456821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>